<commit_message>
feat: add option to set decimal seperator
</commit_message>
<xml_diff>
--- a/examples/test/testFiles/TwoRowsNoErrorsNumberFormats.xlsx
+++ b/examples/test/testFiles/TwoRowsNoErrorsNumberFormats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload/examples/test/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B917BC81-2114-9B49-B45A-29A71EF805C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D4A765-7DE3-BE4F-A964-107581A9AAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="2980" windowWidth="30480" windowHeight="18200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="3240" windowWidth="29160" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID[product_ID]</t>
   </si>
@@ -31,28 +31,32 @@
     <t>UnitPrice[price]</t>
   </si>
   <si>
-    <t>14.99</t>
-  </si>
-  <si>
     <t>1,000.99</t>
   </si>
   <si>
     <t>1.000,99</t>
+  </si>
+  <si>
+    <t>1.000</t>
+  </si>
+  <si>
+    <t>1,000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,16 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -427,138 +424,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>12.56</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>254</v>
-      </c>
-      <c r="B3" s="3">
+        <v>259</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
-        <v>13.68</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>255</v>
-      </c>
-      <c r="B4" s="4">
+        <v>259</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
-        <v>14.88</v>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>256</v>
-      </c>
-      <c r="B5" s="5">
+        <v>259</v>
+      </c>
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
-        <v>14.99</v>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>257</v>
-      </c>
-      <c r="B6" s="6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>258</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>259</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>260</v>
-      </c>
-      <c r="C9" s="8">
-        <v>16.989999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>261</v>
-      </c>
-      <c r="C10" s="8">
-        <v>17.89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>262</v>
-      </c>
-      <c r="C11" s="6">
-        <v>17.5</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>